<commit_message>
Fixing bug of insert file
</commit_message>
<xml_diff>
--- a/InFatec.API/Storage/teste.xlsx
+++ b/InFatec.API/Storage/teste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josea\source\repos\InFatec.API\InFatec.API\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF7C34F-761C-4484-B9ED-3B1104CCFB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CDE325-C9F5-41FA-A290-12944125BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="1590" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="1440" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Segurança da Informação</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Não sei</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de games</t>
+  </si>
+  <si>
+    <t>William Galvão</t>
   </si>
 </sst>
 </file>
@@ -371,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -436,6 +442,23 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>